<commit_message>
Change to Array Sets
</commit_message>
<xml_diff>
--- a/Product Family_familyCtlNetworking/bm_config_attr_sets_familyCtlNetworking.xlsx
+++ b/Product Family_familyCtlNetworking/bm_config_attr_sets_familyCtlNetworking.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="160" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="9460" yWindow="160" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="READ THIS FIRST" sheetId="2" r:id="rId1"/>
     <sheet name="Array Sets" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
   <si>
     <t>Promotions Array (ctlpromotionsArray) </t>
   </si>
@@ -86,6 +87,9 @@
   </si>
   <si>
     <t>This  Excel Workbook Serves as a reference point.   Please add changes observed in the environment</t>
+  </si>
+  <si>
+    <t>dummy</t>
   </si>
 </sst>
 </file>
@@ -525,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -557,10 +561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H22"/>
+  <dimension ref="A3:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -595,6 +599,9 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="30">
+      <c r="A4">
+        <v>1</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -615,6 +622,9 @@
       <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="30">
+      <c r="A6">
+        <v>2</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -635,6 +645,9 @@
       <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="30">
+      <c r="A8">
+        <v>3</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -655,6 +668,9 @@
       <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="30">
+      <c r="A10">
+        <v>4</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
@@ -675,6 +691,9 @@
       <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="30">
+      <c r="A12">
+        <v>5</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
@@ -695,6 +714,9 @@
       <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="30">
+      <c r="A14">
+        <v>6</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
@@ -715,6 +737,9 @@
       <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="30">
+      <c r="A16">
+        <v>7</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -735,6 +760,9 @@
       <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="30">
+      <c r="A18">
+        <v>8</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
@@ -755,6 +783,9 @@
       <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="30">
+      <c r="A20">
+        <v>9</v>
+      </c>
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
@@ -775,6 +806,9 @@
       <c r="A21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="30">
+      <c r="A22">
+        <v>10</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -789,6 +823,14 @@
       </c>
       <c r="F22" s="4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -814,4 +856,26 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="6" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>